<commit_message>
Styrer utsending av melding til formidler fra asset i Orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\TolkFaktura\tolkfakturakundesjekk\TolkFakturaKundesjekk\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\TolkFaktura\tolkfakturakundesjekk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -236,9 +236,6 @@
     <t>S:\F47\NAV_HoT_RPA\RPA-reports\TolkFaktura\logs\Kundesjekk\</t>
   </si>
   <si>
-    <t>Nei</t>
-  </si>
-  <si>
     <t>AssetFormidlerPurring</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
       </rPr>
       <t xml:space="preserve"> (Ja eller Nei)</t>
     </r>
+  </si>
+  <si>
+    <t>Ja</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -768,21 +768,21 @@
         <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>